<commit_message>
added collected results for XPC Cluster and HPC
</commit_message>
<xml_diff>
--- a/src/main/groovy/results/timingData/timings/Collated Timings.xlsx
+++ b/src/main/groovy/results/timingData/timings/Collated Timings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IJGradle\ClusterMandelbrot\src\main\groovy\results\timingData\timings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE5AF2C-6452-4BD7-B38C-89B885EAD2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3861BD9-C020-472E-87A6-1D632DBA2D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19180" yWindow="0" windowWidth="19220" windowHeight="10270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19130" yWindow="100" windowWidth="18910" windowHeight="10570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mean Times" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4560,7 +4559,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4923,7 +4922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD15D1C9-ADF3-4C0E-91CC-AB342DA2E61E}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -5176,7 +5175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4808ACFA-8FAD-47DB-A4EC-9FDF8E989236}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>

</xml_diff>